<commit_message>
WIP in progress error codes.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12347" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39022" uniqueCount="282">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -609,6 +609,312 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId76</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId77</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId78</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IGN ANG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId79</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO ERRORS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COOLANT_SENSOR_FAILURE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coolant temperature sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO_ERROS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO_ERRORS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KNOCKING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Knock detected!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IAT_SENSOR_FAILURE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IAT sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAP_SENSOR_FAILURE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O2_SENSOR_FAILED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O2 sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EGT1_SESNSOR_FAILED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EGT sensor #1 failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EGT2_SENSOR_FAILED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EGT sensor #2 failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EGT_HIGH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EGT too high!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DBW_SENSOR_FAILED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drive by wire failure!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FPR_RELATIVE_ERROR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fuel pressure relative error!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId81</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId82</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
   </si>
 </sst>
 </file>
@@ -3123,6 +3429,280 @@
         <v>58</v>
       </c>
     </row>
+    <row r="58">
+      <c r="B58" t="s">
+        <v>198</v>
+      </c>
+      <c r="C58" t="s">
+        <v>49</v>
+      </c>
+      <c r="D58" t="s">
+        <v>57</v>
+      </c>
+      <c r="E58" t="s">
+        <v>81</v>
+      </c>
+      <c r="F58" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="B59" t="s">
+        <v>199</v>
+      </c>
+      <c r="C59" t="s">
+        <v>49</v>
+      </c>
+      <c r="D59" t="s">
+        <v>80</v>
+      </c>
+      <c r="E59" t="s">
+        <v>129</v>
+      </c>
+      <c r="F59" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="B60" t="s">
+        <v>200</v>
+      </c>
+      <c r="C60" t="s">
+        <v>40</v>
+      </c>
+      <c r="D60" t="s">
+        <v>80</v>
+      </c>
+      <c r="E60" t="s">
+        <v>201</v>
+      </c>
+      <c r="F60" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="B61" t="s">
+        <v>202</v>
+      </c>
+      <c r="C61" t="s">
+        <v>40</v>
+      </c>
+      <c r="D61" t="s">
+        <v>80</v>
+      </c>
+      <c r="E61" t="s">
+        <v>81</v>
+      </c>
+      <c r="F61" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="B62" t="s">
+        <v>204</v>
+      </c>
+      <c r="C62" t="s">
+        <v>40</v>
+      </c>
+      <c r="D62" t="s">
+        <v>80</v>
+      </c>
+      <c r="E62" t="s">
+        <v>203</v>
+      </c>
+      <c r="F62" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="B63" t="s">
+        <v>205</v>
+      </c>
+      <c r="C63" t="s">
+        <v>40</v>
+      </c>
+      <c r="D63" t="s">
+        <v>80</v>
+      </c>
+      <c r="E63" t="s">
+        <v>206</v>
+      </c>
+      <c r="F63" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="B64" t="s">
+        <v>208</v>
+      </c>
+      <c r="C64" t="s">
+        <v>40</v>
+      </c>
+      <c r="D64" t="s">
+        <v>80</v>
+      </c>
+      <c r="E64" t="s">
+        <v>203</v>
+      </c>
+      <c r="F64" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="B65" t="s">
+        <v>209</v>
+      </c>
+      <c r="C65" t="s">
+        <v>40</v>
+      </c>
+      <c r="D65" t="s">
+        <v>80</v>
+      </c>
+      <c r="E65" t="s">
+        <v>210</v>
+      </c>
+      <c r="F65" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="B66" t="s">
+        <v>211</v>
+      </c>
+      <c r="C66" t="s">
+        <v>40</v>
+      </c>
+      <c r="D66" t="s">
+        <v>80</v>
+      </c>
+      <c r="E66" t="s">
+        <v>212</v>
+      </c>
+      <c r="F66" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="B67" t="s">
+        <v>213</v>
+      </c>
+      <c r="C67" t="s">
+        <v>40</v>
+      </c>
+      <c r="D67" t="s">
+        <v>80</v>
+      </c>
+      <c r="E67" t="s">
+        <v>281</v>
+      </c>
+      <c r="F67" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="B68" t="s">
+        <v>215</v>
+      </c>
+      <c r="C68" t="s">
+        <v>40</v>
+      </c>
+      <c r="D68" t="s">
+        <v>80</v>
+      </c>
+      <c r="E68" t="s">
+        <v>216</v>
+      </c>
+      <c r="F68" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="B69" t="s">
+        <v>217</v>
+      </c>
+      <c r="C69" t="s">
+        <v>40</v>
+      </c>
+      <c r="D69" t="s">
+        <v>80</v>
+      </c>
+      <c r="E69" t="s">
+        <v>218</v>
+      </c>
+      <c r="F69" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="B70" t="s">
+        <v>219</v>
+      </c>
+      <c r="C70" t="s">
+        <v>40</v>
+      </c>
+      <c r="D70" t="s">
+        <v>80</v>
+      </c>
+      <c r="E70" t="s">
+        <v>220</v>
+      </c>
+      <c r="F70" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="B71" t="s">
+        <v>221</v>
+      </c>
+      <c r="C71" t="s">
+        <v>40</v>
+      </c>
+      <c r="D71" t="s">
+        <v>80</v>
+      </c>
+      <c r="E71" t="s">
+        <v>222</v>
+      </c>
+      <c r="F71" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="B72" t="s">
+        <v>223</v>
+      </c>
+      <c r="C72" t="s">
+        <v>40</v>
+      </c>
+      <c r="D72" t="s">
+        <v>80</v>
+      </c>
+      <c r="E72" t="s">
+        <v>224</v>
+      </c>
+      <c r="F72" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="B73" t="s">
+        <v>225</v>
+      </c>
+      <c r="C73" t="s">
+        <v>40</v>
+      </c>
+      <c r="D73" t="s">
+        <v>80</v>
+      </c>
+      <c r="E73" t="s">
+        <v>226</v>
+      </c>
+      <c r="F73" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="74"/>
+    <row r="75"/>
   </sheetData>
   <sheetProtection sheet="0" objects="0" scenarios="0" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Version with error messages. Seems there are some bugs.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39022" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56838" uniqueCount="343">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -863,6 +863,221 @@
   <si>
     <t xml:space="preserve">
 MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId83</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId84</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId85</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId86</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boost DC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId87</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId88</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId89</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boost Trgt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId91</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId92</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Injector DC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OIL_TEMPERATURE_PROTECTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oil temperature protection!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OIL_PRESSSURE_PROTECTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oil pressure protection!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLT_PROTECTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLT protection!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FUEL_PRESSURE_PROTECTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fuel pressure protection!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId93</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHECK ENG : &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId94</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENG  PROT : &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId96</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -3593,7 +3808,7 @@
         <v>80</v>
       </c>
       <c r="E67" t="s">
-        <v>281</v>
+        <v>342</v>
       </c>
       <c r="F67" t="s">
         <v>58</v>
@@ -3701,8 +3916,346 @@
         <v>58</v>
       </c>
     </row>
-    <row r="74"/>
-    <row r="75"/>
+    <row r="74">
+      <c r="B74" t="s">
+        <v>229</v>
+      </c>
+      <c r="C74" t="s">
+        <v>49</v>
+      </c>
+      <c r="D74" t="s">
+        <v>57</v>
+      </c>
+      <c r="E74" t="s">
+        <v>81</v>
+      </c>
+      <c r="F74" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="B75" t="s">
+        <v>230</v>
+      </c>
+      <c r="C75" t="s">
+        <v>49</v>
+      </c>
+      <c r="D75" t="s">
+        <v>80</v>
+      </c>
+      <c r="E75" t="s">
+        <v>129</v>
+      </c>
+      <c r="F75" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="B76" t="s">
+        <v>283</v>
+      </c>
+      <c r="C76" t="s">
+        <v>40</v>
+      </c>
+      <c r="D76" t="s">
+        <v>80</v>
+      </c>
+      <c r="E76" t="s">
+        <v>284</v>
+      </c>
+      <c r="F76" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="B77" t="s">
+        <v>285</v>
+      </c>
+      <c r="C77" t="s">
+        <v>49</v>
+      </c>
+      <c r="D77" t="s">
+        <v>57</v>
+      </c>
+      <c r="E77" t="s">
+        <v>81</v>
+      </c>
+      <c r="F77" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="B78" t="s">
+        <v>286</v>
+      </c>
+      <c r="C78" t="s">
+        <v>49</v>
+      </c>
+      <c r="D78" t="s">
+        <v>80</v>
+      </c>
+      <c r="E78" t="s">
+        <v>129</v>
+      </c>
+      <c r="F78" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="B79" t="s">
+        <v>287</v>
+      </c>
+      <c r="C79" t="s">
+        <v>40</v>
+      </c>
+      <c r="D79" t="s">
+        <v>80</v>
+      </c>
+      <c r="E79" t="s">
+        <v>288</v>
+      </c>
+      <c r="F79" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="B80" t="s">
+        <v>289</v>
+      </c>
+      <c r="C80" t="s">
+        <v>49</v>
+      </c>
+      <c r="D80" t="s">
+        <v>57</v>
+      </c>
+      <c r="E80" t="s">
+        <v>81</v>
+      </c>
+      <c r="F80" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="B81" t="s">
+        <v>290</v>
+      </c>
+      <c r="C81" t="s">
+        <v>49</v>
+      </c>
+      <c r="D81" t="s">
+        <v>80</v>
+      </c>
+      <c r="E81" t="s">
+        <v>129</v>
+      </c>
+      <c r="F81" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="B82" t="s">
+        <v>291</v>
+      </c>
+      <c r="C82" t="s">
+        <v>40</v>
+      </c>
+      <c r="D82" t="s">
+        <v>80</v>
+      </c>
+      <c r="E82" t="s">
+        <v>292</v>
+      </c>
+      <c r="F82" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="B83" t="s">
+        <v>293</v>
+      </c>
+      <c r="C83" t="s">
+        <v>49</v>
+      </c>
+      <c r="D83" t="s">
+        <v>57</v>
+      </c>
+      <c r="E83" t="s">
+        <v>81</v>
+      </c>
+      <c r="F83" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="B84" t="s">
+        <v>294</v>
+      </c>
+      <c r="C84" t="s">
+        <v>49</v>
+      </c>
+      <c r="D84" t="s">
+        <v>80</v>
+      </c>
+      <c r="E84" t="s">
+        <v>129</v>
+      </c>
+      <c r="F84" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="B85" t="s">
+        <v>295</v>
+      </c>
+      <c r="C85" t="s">
+        <v>40</v>
+      </c>
+      <c r="D85" t="s">
+        <v>80</v>
+      </c>
+      <c r="E85" t="s">
+        <v>296</v>
+      </c>
+      <c r="F85" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="B86" t="s">
+        <v>307</v>
+      </c>
+      <c r="C86" t="s">
+        <v>40</v>
+      </c>
+      <c r="D86" t="s">
+        <v>80</v>
+      </c>
+      <c r="E86" t="s">
+        <v>308</v>
+      </c>
+      <c r="F86" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="B87" t="s">
+        <v>309</v>
+      </c>
+      <c r="C87" t="s">
+        <v>40</v>
+      </c>
+      <c r="D87" t="s">
+        <v>80</v>
+      </c>
+      <c r="E87" t="s">
+        <v>310</v>
+      </c>
+      <c r="F87" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="B88" t="s">
+        <v>311</v>
+      </c>
+      <c r="C88" t="s">
+        <v>40</v>
+      </c>
+      <c r="D88" t="s">
+        <v>80</v>
+      </c>
+      <c r="E88" t="s">
+        <v>312</v>
+      </c>
+      <c r="F88" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="B89" t="s">
+        <v>313</v>
+      </c>
+      <c r="C89" t="s">
+        <v>40</v>
+      </c>
+      <c r="D89" t="s">
+        <v>80</v>
+      </c>
+      <c r="E89" t="s">
+        <v>314</v>
+      </c>
+      <c r="F89" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="B90" t="s">
+        <v>321</v>
+      </c>
+      <c r="C90" t="s">
+        <v>40</v>
+      </c>
+      <c r="D90" t="s">
+        <v>80</v>
+      </c>
+      <c r="E90" t="s">
+        <v>322</v>
+      </c>
+      <c r="F90" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="B91" t="s">
+        <v>323</v>
+      </c>
+      <c r="C91" t="s">
+        <v>40</v>
+      </c>
+      <c r="D91" t="s">
+        <v>80</v>
+      </c>
+      <c r="E91" t="s">
+        <v>324</v>
+      </c>
+      <c r="F91" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="B92" t="s">
+        <v>327</v>
+      </c>
+      <c r="C92" t="s">
+        <v>40</v>
+      </c>
+      <c r="D92" t="s">
+        <v>80</v>
+      </c>
+      <c r="E92" t="s">
+        <v>328</v>
+      </c>
+      <c r="F92" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="B93" t="s">
+        <v>329</v>
+      </c>
+      <c r="C93" t="s">
+        <v>40</v>
+      </c>
+      <c r="D93" t="s">
+        <v>80</v>
+      </c>
+      <c r="E93" t="s">
+        <v>324</v>
+      </c>
+      <c r="F93" t="s">
+        <v>58</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection sheet="0" objects="0" scenarios="0" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Removed error logic from main screen. Should understand got EMU errors work.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56838" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57433" uniqueCount="347">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1130,6 +1130,18 @@
   <si>
     <t xml:space="preserve">
 MAP sensor failed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId97</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId98</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KM/H</t>
   </si>
 </sst>
 </file>
@@ -3808,7 +3820,7 @@
         <v>80</v>
       </c>
       <c r="E67" t="s">
-        <v>342</v>
+        <v>214</v>
       </c>
       <c r="F67" t="s">
         <v>58</v>
@@ -4253,6 +4265,57 @@
         <v>324</v>
       </c>
       <c r="F93" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="B94" t="s">
+        <v>343</v>
+      </c>
+      <c r="C94" t="s">
+        <v>49</v>
+      </c>
+      <c r="D94" t="s">
+        <v>57</v>
+      </c>
+      <c r="E94" t="s">
+        <v>81</v>
+      </c>
+      <c r="F94" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="B95" t="s">
+        <v>344</v>
+      </c>
+      <c r="C95" t="s">
+        <v>49</v>
+      </c>
+      <c r="D95" t="s">
+        <v>80</v>
+      </c>
+      <c r="E95" t="s">
+        <v>161</v>
+      </c>
+      <c r="F95" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="B96" t="s">
+        <v>345</v>
+      </c>
+      <c r="C96" t="s">
+        <v>40</v>
+      </c>
+      <c r="D96" t="s">
+        <v>80</v>
+      </c>
+      <c r="E96" t="s">
+        <v>346</v>
+      </c>
+      <c r="F96" t="s">
         <v>58</v>
       </c>
     </row>

</xml_diff>